<commit_message>
Remove script de limpeza e finaliza ajustes
</commit_message>
<xml_diff>
--- a/fornecedores.xlsx
+++ b/fornecedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tenda0-my.sharepoint.com/personal/daniela_monteiro_tenda_com/Documents/Imagens/Danny/Projeto S-Ponto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B97FF18-301D-4886-81C3-067F6DC3A910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1B97FF18-301D-4886-81C3-067F6DC3A910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D01C2573-361B-4CC0-B960-6AA478468D09}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Endereço</t>
+    <t>Endereco</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A1:F1838"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:F1838"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>